<commit_message>
start data analysis 4 chmielewskii genotypes
</commit_message>
<xml_diff>
--- a/Fig.1_Screen_4_chmielewskiis/metadata.xlsx
+++ b/Fig.1_Screen_4_chmielewskiis/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lissydenkers/Documents/chapters/chm/data/bioassay 4 chmielewskiis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisde\OneDrive\Documents\GitHub\Riboflavin\Fig.1_Screen_4_chmielewskiis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7423A9-355D-644D-BCE6-C18D256500DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F76488-7BAE-49CD-804F-5FE4BCAE508F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12060" yWindow="520" windowWidth="24960" windowHeight="17780" activeTab="2" xr2:uid="{2CBDDDEE-8A29-412C-B313-79E53312EB71}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2CBDDDEE-8A29-412C-B313-79E53312EB71}"/>
   </bookViews>
   <sheets>
     <sheet name="Explenations of columns" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="87">
   <si>
     <t>genotype</t>
   </si>
@@ -331,25 +331,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -360,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,14 +668,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -699,7 +686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -710,7 +697,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -721,7 +708,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -732,7 +719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -743,7 +730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -754,7 +741,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -765,7 +752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -776,7 +763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -787,7 +774,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -798,7 +785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -809,7 +796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -820,7 +807,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -841,17 +828,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A04CE23-C750-45D4-B9FA-23E4C654D1EE}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D51"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -868,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -885,7 +872,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -902,7 +889,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -919,7 +906,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -936,7 +923,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -953,7 +940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -970,7 +957,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -987,7 +974,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1004,7 +991,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1021,7 +1008,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -1038,7 +1025,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1055,7 +1042,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1072,7 +1059,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1089,7 +1076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -1106,7 +1093,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -1123,7 +1110,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1140,7 +1127,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1157,7 +1144,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1174,7 +1161,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1191,7 +1178,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1208,7 +1195,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1225,7 +1212,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1242,7 +1229,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -1259,7 +1246,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1276,7 +1263,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -1293,7 +1280,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1310,7 +1297,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1327,7 +1314,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -1344,7 +1331,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -1361,7 +1348,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1378,7 +1365,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1395,7 +1382,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1412,7 +1399,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1429,7 +1416,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -1446,7 +1433,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -1463,7 +1450,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -1480,7 +1467,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -1494,10 +1481,10 @@
         <v>45015</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -1511,10 +1498,10 @@
         <v>45015</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -1531,7 +1518,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -1548,7 +1535,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -1565,7 +1552,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>65</v>
       </c>
@@ -1582,7 +1569,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -1599,7 +1586,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -1616,7 +1603,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -1633,7 +1620,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -1650,7 +1637,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -1667,7 +1654,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -1684,7 +1671,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -1701,444 +1688,439 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D51" s="1">
-        <v>45015</v>
-      </c>
-      <c r="E51" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D121" s="1"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D125" s="1"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D126" s="1"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D128" s="1"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D129" s="1"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D130" s="1"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D131" s="1"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D132" s="1"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D133" s="1"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D134" s="1"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D135" s="1"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D136" s="1"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D137" s="1"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D142" s="1"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D143" s="1"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D144" s="1"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D145" s="1"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D146" s="1"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D147" s="1"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D148" s="1"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D149" s="1"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D150" s="1"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D151" s="1"/>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D152" s="1"/>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D154" s="1"/>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D155" s="1"/>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D158" s="1"/>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D159" s="1"/>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D161" s="1"/>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D162" s="1"/>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D163" s="1"/>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D164" s="1"/>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D165" s="1"/>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D166" s="1"/>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D167" s="1"/>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D168" s="1"/>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D169" s="1"/>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D171" s="1"/>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D172" s="1"/>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D173" s="1"/>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D174" s="1"/>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D175" s="1"/>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D176" s="1"/>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D177" s="1"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D178" s="1"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D179" s="1"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D180" s="1"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D181" s="1"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D182" s="1"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D183" s="1"/>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D184" s="1"/>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D185" s="1"/>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D186" s="1"/>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D187" s="1"/>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D188" s="1"/>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D189" s="1"/>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D190" s="1"/>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D191" s="1"/>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D192" s="1"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D193" s="1"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D194" s="1"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D195" s="1"/>
     </row>
   </sheetData>
@@ -2151,22 +2133,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDF49D4-CA04-40EF-A535-8F15759A0706}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2174,18 +2156,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2193,7 +2175,7 @@
         <v>44987</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2201,7 +2183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2209,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -2217,7 +2199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2225,7 +2207,7 @@
         <v>44988</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2233,7 +2215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2241,7 +2223,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2249,7 +2231,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2257,7 +2239,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2265,7 +2247,7 @@
         <v>44991</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2273,7 +2255,7 @@
         <v>45015</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>

</xml_diff>